<commit_message>
Cohorts updates with Revised Keypop
</commit_message>
<xml_diff>
--- a/web/pns/ART_Daily_Form_v800_2021_11_25_.xlsx
+++ b/web/pns/ART_Daily_Form_v800_2021_11_25_.xlsx
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="CC71" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="400"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pmtct" sheetId="13" r:id="rId1"/>
     <sheet name="ccc" sheetId="14" r:id="rId2"/>
-    <sheet name="non-hiv" sheetId="15" r:id="rId3"/>
+    <sheet name="TB ACF" sheetId="15" r:id="rId3"/>
     <sheet name="data" sheetId="9" state="hidden" r:id="rId4"/>
     <sheet name="SiteSetUp" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="SurgeSites" sheetId="8" state="hidden" r:id="rId6"/>
@@ -25,44 +25,44 @@
     <definedName name="Baringo">SiteSetUp!$B$2:$B$29</definedName>
     <definedName name="County">SiteSetUp!$A$2:$A$5</definedName>
     <definedName name="dd" localSheetId="1">ccc!$F$5</definedName>
-    <definedName name="dd" localSheetId="2">'non-hiv'!$F$5</definedName>
     <definedName name="dd" localSheetId="0">pmtct!$F$5</definedName>
+    <definedName name="dd" localSheetId="2">'TB ACF'!$F$5</definedName>
     <definedName name="dd">#REF!</definedName>
     <definedName name="Kajiado" localSheetId="2">SiteSetUp!#REF!</definedName>
     <definedName name="Kajiado">SiteSetUp!#REF!</definedName>
     <definedName name="Laikipia">SiteSetUp!$C$2:$C$33</definedName>
     <definedName name="mflcode" localSheetId="1">ccc!$C$5</definedName>
-    <definedName name="mflcode" localSheetId="2">'non-hiv'!$C$5</definedName>
     <definedName name="mflcode" localSheetId="0">pmtct!$C$5</definedName>
+    <definedName name="mflcode" localSheetId="2">'TB ACF'!$C$5</definedName>
     <definedName name="mflcode">#REF!</definedName>
     <definedName name="mm" localSheetId="1">ccc!$G$5</definedName>
-    <definedName name="mm" localSheetId="2">'non-hiv'!$G$5</definedName>
     <definedName name="mm" localSheetId="0">pmtct!$G$5</definedName>
+    <definedName name="mm" localSheetId="2">'TB ACF'!$G$5</definedName>
     <definedName name="mm">#REF!</definedName>
     <definedName name="Nakuru">SiteSetUp!$D$2:$D$171</definedName>
     <definedName name="Narok" localSheetId="2">SiteSetUp!#REF!</definedName>
     <definedName name="Narok">SiteSetUp!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">ccc!$A$2:$AB$57</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'non-hiv'!$A$2:$AA$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">pmtct!$A$2:$AA$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'TB ACF'!$A$2:$AA$42</definedName>
     <definedName name="Samburu">SiteSetUp!$E$2:$E$24</definedName>
     <definedName name="sdp" localSheetId="1">ccc!$C$6</definedName>
-    <definedName name="sdp" localSheetId="2">'non-hiv'!$C$6</definedName>
     <definedName name="sdp" localSheetId="0">pmtct!$C$6</definedName>
+    <definedName name="sdp" localSheetId="2">'TB ACF'!$C$6</definedName>
     <definedName name="sdp">#REF!</definedName>
     <definedName name="site" localSheetId="1">ccc!$B$5</definedName>
-    <definedName name="site" localSheetId="2">'non-hiv'!$B$5</definedName>
     <definedName name="site" localSheetId="0">pmtct!$B$5</definedName>
+    <definedName name="site" localSheetId="2">'TB ACF'!$B$5</definedName>
     <definedName name="site">#REF!</definedName>
     <definedName name="sitecounty" localSheetId="1">ccc!$B$3</definedName>
-    <definedName name="sitecounty" localSheetId="2">'non-hiv'!$B$3</definedName>
     <definedName name="sitecounty" localSheetId="0">pmtct!$B$3</definedName>
+    <definedName name="sitecounty" localSheetId="2">'TB ACF'!$B$3</definedName>
     <definedName name="sitecounty">#REF!</definedName>
     <definedName name="Turkana" localSheetId="2">SiteSetUp!#REF!</definedName>
     <definedName name="Turkana">SiteSetUp!#REF!</definedName>
     <definedName name="yyyy" localSheetId="1">ccc!$H$5</definedName>
-    <definedName name="yyyy" localSheetId="2">'non-hiv'!$H$5</definedName>
     <definedName name="yyyy" localSheetId="0">pmtct!$H$5</definedName>
+    <definedName name="yyyy" localSheetId="2">'TB ACF'!$H$5</definedName>
     <definedName name="yyyy">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="871">
   <si>
     <t>F</t>
   </si>
@@ -2756,6 +2756,18 @@
   </si>
   <si>
     <t>Total Dispensary_16403</t>
+  </si>
+  <si>
+    <t>Non-HIV Patients Screened for TB (ACF)</t>
+  </si>
+  <si>
+    <t>No of confirmed TB presumptive cases at TB clinic</t>
+  </si>
+  <si>
+    <t>No of TB presumptive with samples collected for TB investigative work up (gene expert testing and any other diagnostic)</t>
+  </si>
+  <si>
+    <t>No of TB presumptive cases diagnosed to have active TB (TB positive)</t>
   </si>
 </sst>
 </file>
@@ -3741,6 +3753,78 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3780,86 +3864,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9791,7 +9803,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>4517</xdr:colOff>
+      <xdr:colOff>4516</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>143125</xdr:rowOff>
     </xdr:to>
@@ -9838,7 +9850,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>278640</xdr:colOff>
+      <xdr:colOff>278641</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>103101</xdr:rowOff>
     </xdr:to>
@@ -10121,7 +10133,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>264061</xdr:colOff>
+      <xdr:colOff>264062</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>98242</xdr:rowOff>
     </xdr:to>
@@ -10506,31 +10518,31 @@
   </sheetPr>
   <dimension ref="A1:CB69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="71" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="71" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Y45" sqref="Y45"/>
       <selection pane="topRight" activeCell="Y45" sqref="Y45"/>
       <selection pane="bottomLeft" activeCell="Y45" sqref="Y45"/>
-      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
+      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="11.65"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.3984375" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="23" width="3.86328125" style="26" customWidth="1"/>
-    <col min="24" max="24" width="5.1328125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="3.85546875" style="26" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" style="26" customWidth="1"/>
     <col min="25" max="25" width="5" style="26" customWidth="1"/>
-    <col min="26" max="26" width="6.265625" style="26" customWidth="1"/>
-    <col min="27" max="27" width="4.265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" style="26" customWidth="1"/>
+    <col min="27" max="27" width="4.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="26" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="57.73046875" style="27" customWidth="1"/>
-    <col min="30" max="30" width="4.3984375" style="27" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="57.7109375" style="27" customWidth="1"/>
+    <col min="30" max="30" width="4.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="31" max="61" width="3" style="27" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="6.59765625" style="27"/>
+    <col min="62" max="16384" width="6.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="12" thickBot="1">
+    <row r="1" spans="1:80" ht="12.75" thickBot="1">
       <c r="A1" s="23"/>
       <c r="B1" s="24"/>
       <c r="C1" s="25"/>
@@ -10655,8 +10667,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="2" spans="1:80" ht="12" thickBot="1">
-      <c r="A2" s="92" t="s">
+    <row r="2" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A2" s="115" t="s">
         <v>856</v>
       </c>
       <c r="B2" s="67" t="s">
@@ -10746,8 +10758,8 @@
       <c r="BH2" s="74"/>
       <c r="BI2" s="74"/>
     </row>
-    <row r="3" spans="1:80" ht="12" thickBot="1">
-      <c r="A3" s="93"/>
+    <row r="3" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A3" s="116"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34"/>
@@ -10776,15 +10788,15 @@
       <c r="AA3" s="36"/>
     </row>
     <row r="4" spans="1:80">
-      <c r="A4" s="93"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -10803,42 +10815,42 @@
       <c r="U4" s="37"/>
       <c r="V4" s="37"/>
       <c r="W4" s="38"/>
-      <c r="X4" s="97" t="s">
+      <c r="X4" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="98"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="121"/>
       <c r="AA4" s="39"/>
     </row>
-    <row r="5" spans="1:80" ht="12" thickBot="1">
-      <c r="A5" s="94"/>
+    <row r="5" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A5" s="117"/>
       <c r="B5" s="40"/>
-      <c r="C5" s="99" t="str">
+      <c r="C5" s="122" t="str">
         <f>IF(ISERROR((RIGHT(B5,LEN(B5)- FIND("_",B5)))),"",(RIGHT(B5,LEN(B5)- FIND("_",B5))))</f>
         <v/>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102" t="s">
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125" t="s">
         <v>807</v>
       </c>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="104"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="126"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="127"/>
       <c r="X5" s="41" t="s">
         <v>4</v>
       </c>
@@ -10850,7 +10862,7 @@
       </c>
       <c r="AA5" s="43"/>
     </row>
-    <row r="6" spans="1:80" ht="12" thickBot="1">
+    <row r="6" spans="1:80" ht="12.75" thickBot="1">
       <c r="A6" s="44"/>
       <c r="B6" s="45" t="s">
         <v>161</v>
@@ -10884,50 +10896,50 @@
       <c r="AA6" s="105"/>
     </row>
     <row r="7" spans="1:80" s="48" customFormat="1">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="106" t="s">
         <v>193</v>
       </c>
       <c r="D7" s="106"/>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="103" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="107" t="s">
+      <c r="F7" s="104"/>
+      <c r="G7" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="115"/>
-      <c r="I7" s="107" t="s">
+      <c r="H7" s="104"/>
+      <c r="I7" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="115"/>
-      <c r="K7" s="107" t="s">
+      <c r="J7" s="104"/>
+      <c r="K7" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="115"/>
-      <c r="M7" s="107" t="s">
+      <c r="L7" s="104"/>
+      <c r="M7" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="107" t="s">
+      <c r="N7" s="110"/>
+      <c r="O7" s="103" t="s">
         <v>199</v>
       </c>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="107" t="s">
+      <c r="P7" s="104"/>
+      <c r="Q7" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="114"/>
+      <c r="R7" s="110"/>
       <c r="S7" s="106" t="s">
         <v>201</v>
       </c>
       <c r="T7" s="106"/>
-      <c r="U7" s="107" t="s">
+      <c r="U7" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="V7" s="115"/>
+      <c r="V7" s="104"/>
       <c r="W7" s="106" t="s">
         <v>203</v>
       </c>
@@ -10935,8 +10947,8 @@
       <c r="Y7" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="123" t="s">
+      <c r="Z7" s="103"/>
+      <c r="AA7" s="98" t="s">
         <v>216</v>
       </c>
       <c r="AB7" s="46"/>
@@ -10993,9 +11005,9 @@
       <c r="CA7" s="47"/>
       <c r="CB7" s="47"/>
     </row>
-    <row r="8" spans="1:80" s="48" customFormat="1" ht="12" thickBot="1">
-      <c r="A8" s="118"/>
-      <c r="B8" s="119"/>
+    <row r="8" spans="1:80" s="48" customFormat="1" ht="12.75" thickBot="1">
+      <c r="A8" s="113"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="49" t="s">
         <v>0</v>
       </c>
@@ -11068,7 +11080,7 @@
       <c r="Z8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AA8" s="124"/>
+      <c r="AA8" s="99"/>
       <c r="AB8" s="46"/>
       <c r="AC8" s="27"/>
       <c r="AD8" s="47"/>
@@ -11123,38 +11135,38 @@
       <c r="CA8" s="47"/>
       <c r="CB8" s="47"/>
     </row>
-    <row r="9" spans="1:80" s="48" customFormat="1" ht="14.25" thickBot="1">
+    <row r="9" spans="1:80" s="48" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="109"/>
-      <c r="Q9" s="109"/>
-      <c r="R9" s="109"/>
-      <c r="S9" s="109"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="109"/>
-      <c r="V9" s="109"/>
-      <c r="W9" s="109"/>
-      <c r="X9" s="109"/>
-      <c r="Y9" s="109"/>
-      <c r="Z9" s="109"/>
-      <c r="AA9" s="110"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108"/>
+      <c r="U9" s="108"/>
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="108"/>
+      <c r="Y9" s="108"/>
+      <c r="Z9" s="108"/>
+      <c r="AA9" s="109"/>
       <c r="AB9" s="53" t="s">
         <v>207</v>
       </c>
@@ -11450,7 +11462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:80" ht="12" thickBot="1">
+    <row r="16" spans="1:80" ht="12.75" thickBot="1">
       <c r="A16" s="54">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -11490,36 +11502,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="59" customFormat="1" ht="14.25" thickBot="1">
+    <row r="17" spans="1:29" s="59" customFormat="1" ht="15.75" thickBot="1">
       <c r="A17" s="54"/>
-      <c r="B17" s="111" t="s">
+      <c r="B17" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="112"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="112"/>
-      <c r="Y17" s="112"/>
-      <c r="Z17" s="112"/>
-      <c r="AA17" s="113"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="93"/>
+      <c r="V17" s="93"/>
+      <c r="W17" s="93"/>
+      <c r="X17" s="93"/>
+      <c r="Y17" s="93"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="94"/>
       <c r="AB17" s="58" t="s">
         <v>18</v>
       </c>
@@ -11605,7 +11617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="12" thickBot="1">
+    <row r="20" spans="1:29" ht="12.75" thickBot="1">
       <c r="A20" s="54">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -11645,36 +11657,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="14.25" thickBot="1">
+    <row r="21" spans="1:29" ht="15.75" thickBot="1">
       <c r="A21" s="54"/>
-      <c r="B21" s="111" t="s">
+      <c r="B21" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
-      <c r="N21" s="112"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="112"/>
-      <c r="Q21" s="112"/>
-      <c r="R21" s="112"/>
-      <c r="S21" s="112"/>
-      <c r="T21" s="112"/>
-      <c r="U21" s="112"/>
-      <c r="V21" s="112"/>
-      <c r="W21" s="112"/>
-      <c r="X21" s="112"/>
-      <c r="Y21" s="112"/>
-      <c r="Z21" s="112"/>
-      <c r="AA21" s="113"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="93"/>
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="93"/>
+      <c r="W21" s="93"/>
+      <c r="X21" s="93"/>
+      <c r="Y21" s="93"/>
+      <c r="Z21" s="93"/>
+      <c r="AA21" s="94"/>
       <c r="AB21" s="60" t="s">
         <v>17</v>
       </c>
@@ -12078,7 +12090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="12" thickBot="1">
+    <row r="32" spans="1:29" ht="12.75" thickBot="1">
       <c r="A32" s="54">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -12118,36 +12130,36 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="14.25" thickBot="1">
+    <row r="33" spans="1:28" ht="15.75" thickBot="1">
       <c r="A33" s="54"/>
-      <c r="B33" s="111" t="s">
+      <c r="B33" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="112"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
-      <c r="K33" s="112"/>
-      <c r="L33" s="112"/>
-      <c r="M33" s="112"/>
-      <c r="N33" s="112"/>
-      <c r="O33" s="112"/>
-      <c r="P33" s="112"/>
-      <c r="Q33" s="112"/>
-      <c r="R33" s="112"/>
-      <c r="S33" s="112"/>
-      <c r="T33" s="112"/>
-      <c r="U33" s="112"/>
-      <c r="V33" s="112"/>
-      <c r="W33" s="112"/>
-      <c r="X33" s="112"/>
-      <c r="Y33" s="112"/>
-      <c r="Z33" s="112"/>
-      <c r="AA33" s="113"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="93"/>
+      <c r="V33" s="93"/>
+      <c r="W33" s="93"/>
+      <c r="X33" s="93"/>
+      <c r="Y33" s="93"/>
+      <c r="Z33" s="93"/>
+      <c r="AA33" s="94"/>
       <c r="AB33" s="60" t="s">
         <v>15</v>
       </c>
@@ -12191,7 +12203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="12" thickBot="1">
+    <row r="35" spans="1:28" ht="12.75" thickBot="1">
       <c r="A35" s="54">
         <f t="shared" ref="A35" si="4">IF(ISERROR((A34+1)),"",(A34+1))</f>
         <v>23</v>
@@ -12231,36 +12243,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="14.25" thickBot="1">
+    <row r="36" spans="1:28" ht="15.75" thickBot="1">
       <c r="A36" s="54"/>
-      <c r="B36" s="111" t="s">
+      <c r="B36" s="92" t="s">
         <v>757</v>
       </c>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="112"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="112"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="112"/>
-      <c r="M36" s="112"/>
-      <c r="N36" s="112"/>
-      <c r="O36" s="112"/>
-      <c r="P36" s="112"/>
-      <c r="Q36" s="112"/>
-      <c r="R36" s="112"/>
-      <c r="S36" s="112"/>
-      <c r="T36" s="112"/>
-      <c r="U36" s="112"/>
-      <c r="V36" s="112"/>
-      <c r="W36" s="112"/>
-      <c r="X36" s="112"/>
-      <c r="Y36" s="112"/>
-      <c r="Z36" s="112"/>
-      <c r="AA36" s="113"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="93"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="93"/>
+      <c r="O36" s="93"/>
+      <c r="P36" s="93"/>
+      <c r="Q36" s="93"/>
+      <c r="R36" s="93"/>
+      <c r="S36" s="93"/>
+      <c r="T36" s="93"/>
+      <c r="U36" s="93"/>
+      <c r="V36" s="93"/>
+      <c r="W36" s="93"/>
+      <c r="X36" s="93"/>
+      <c r="Y36" s="93"/>
+      <c r="Z36" s="93"/>
+      <c r="AA36" s="94"/>
       <c r="AB36" s="56" t="s">
         <v>758</v>
       </c>
@@ -12304,36 +12316,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="14.25" thickBot="1">
+    <row r="38" spans="1:28" ht="15.75" thickBot="1">
       <c r="A38" s="54"/>
-      <c r="B38" s="111" t="s">
+      <c r="B38" s="92" t="s">
         <v>761</v>
       </c>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="112"/>
-      <c r="N38" s="112"/>
-      <c r="O38" s="112"/>
-      <c r="P38" s="112"/>
-      <c r="Q38" s="112"/>
-      <c r="R38" s="112"/>
-      <c r="S38" s="112"/>
-      <c r="T38" s="112"/>
-      <c r="U38" s="112"/>
-      <c r="V38" s="112"/>
-      <c r="W38" s="112"/>
-      <c r="X38" s="112"/>
-      <c r="Y38" s="112"/>
-      <c r="Z38" s="112"/>
-      <c r="AA38" s="113"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="93"/>
+      <c r="O38" s="93"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="93"/>
+      <c r="T38" s="93"/>
+      <c r="U38" s="93"/>
+      <c r="V38" s="93"/>
+      <c r="W38" s="93"/>
+      <c r="X38" s="93"/>
+      <c r="Y38" s="93"/>
+      <c r="Z38" s="93"/>
+      <c r="AA38" s="94"/>
       <c r="AB38" s="56" t="s">
         <v>0</v>
       </c>
@@ -12497,7 +12509,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="12" thickBot="1">
+    <row r="43" spans="1:28" ht="12.75" thickBot="1">
       <c r="A43" s="54">
         <v>29</v>
       </c>
@@ -12536,36 +12548,36 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="14.25" thickBot="1">
+    <row r="44" spans="1:28" ht="15.75" thickBot="1">
       <c r="A44" s="54"/>
-      <c r="B44" s="111" t="s">
+      <c r="B44" s="92" t="s">
         <v>801</v>
       </c>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="112"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
-      <c r="K44" s="112"/>
-      <c r="L44" s="112"/>
-      <c r="M44" s="112"/>
-      <c r="N44" s="112"/>
-      <c r="O44" s="112"/>
-      <c r="P44" s="112"/>
-      <c r="Q44" s="112"/>
-      <c r="R44" s="112"/>
-      <c r="S44" s="112"/>
-      <c r="T44" s="112"/>
-      <c r="U44" s="112"/>
-      <c r="V44" s="112"/>
-      <c r="W44" s="112"/>
-      <c r="X44" s="112"/>
-      <c r="Y44" s="112"/>
-      <c r="Z44" s="112"/>
-      <c r="AA44" s="113"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="94"/>
       <c r="AB44" s="56" t="s">
         <v>802</v>
       </c>
@@ -12648,7 +12660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="12" thickBot="1">
+    <row r="47" spans="1:28" ht="12.75" thickBot="1">
       <c r="A47" s="54">
         <v>32</v>
       </c>
@@ -12687,36 +12699,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="14.25" thickBot="1">
+    <row r="48" spans="1:28" ht="15.75" thickBot="1">
       <c r="A48" s="54"/>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="92" t="s">
         <v>810</v>
       </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="M48" s="112"/>
-      <c r="N48" s="112"/>
-      <c r="O48" s="112"/>
-      <c r="P48" s="112"/>
-      <c r="Q48" s="112"/>
-      <c r="R48" s="112"/>
-      <c r="S48" s="112"/>
-      <c r="T48" s="112"/>
-      <c r="U48" s="112"/>
-      <c r="V48" s="112"/>
-      <c r="W48" s="112"/>
-      <c r="X48" s="112"/>
-      <c r="Y48" s="112"/>
-      <c r="Z48" s="112"/>
-      <c r="AA48" s="113"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="93"/>
+      <c r="P48" s="93"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="93"/>
+      <c r="T48" s="93"/>
+      <c r="U48" s="93"/>
+      <c r="V48" s="93"/>
+      <c r="W48" s="93"/>
+      <c r="X48" s="93"/>
+      <c r="Y48" s="93"/>
+      <c r="Z48" s="93"/>
+      <c r="AA48" s="94"/>
       <c r="AB48" s="56" t="s">
         <v>814</v>
       </c>
@@ -12799,7 +12811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="12" thickBot="1">
+    <row r="51" spans="1:28" ht="12.75" thickBot="1">
       <c r="A51" s="54">
         <v>35</v>
       </c>
@@ -12838,36 +12850,36 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="14.25" thickBot="1">
+    <row r="52" spans="1:28" ht="15.75" thickBot="1">
       <c r="A52" s="54"/>
-      <c r="B52" s="111" t="s">
+      <c r="B52" s="92" t="s">
         <v>821</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="112"/>
-      <c r="L52" s="112"/>
-      <c r="M52" s="112"/>
-      <c r="N52" s="112"/>
-      <c r="O52" s="112"/>
-      <c r="P52" s="112"/>
-      <c r="Q52" s="112"/>
-      <c r="R52" s="112"/>
-      <c r="S52" s="112"/>
-      <c r="T52" s="112"/>
-      <c r="U52" s="112"/>
-      <c r="V52" s="112"/>
-      <c r="W52" s="112"/>
-      <c r="X52" s="112"/>
-      <c r="Y52" s="112"/>
-      <c r="Z52" s="112"/>
-      <c r="AA52" s="113"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
+      <c r="K52" s="93"/>
+      <c r="L52" s="93"/>
+      <c r="M52" s="93"/>
+      <c r="N52" s="93"/>
+      <c r="O52" s="93"/>
+      <c r="P52" s="93"/>
+      <c r="Q52" s="93"/>
+      <c r="R52" s="93"/>
+      <c r="S52" s="93"/>
+      <c r="T52" s="93"/>
+      <c r="U52" s="93"/>
+      <c r="V52" s="93"/>
+      <c r="W52" s="93"/>
+      <c r="X52" s="93"/>
+      <c r="Y52" s="93"/>
+      <c r="Z52" s="93"/>
+      <c r="AA52" s="94"/>
       <c r="AB52" s="56" t="s">
         <v>820</v>
       </c>
@@ -12950,36 +12962,36 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="55" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A55" s="54"/>
-      <c r="B55" s="111" t="s">
+      <c r="B55" s="92" t="s">
         <v>818</v>
       </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="112"/>
-      <c r="L55" s="112"/>
-      <c r="M55" s="112"/>
-      <c r="N55" s="112"/>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
-      <c r="Q55" s="112"/>
-      <c r="R55" s="112"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="112"/>
-      <c r="U55" s="112"/>
-      <c r="V55" s="112"/>
-      <c r="W55" s="112"/>
-      <c r="X55" s="112"/>
-      <c r="Y55" s="112"/>
-      <c r="Z55" s="112"/>
-      <c r="AA55" s="113"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="93"/>
+      <c r="J55" s="93"/>
+      <c r="K55" s="93"/>
+      <c r="L55" s="93"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="93"/>
+      <c r="O55" s="93"/>
+      <c r="P55" s="93"/>
+      <c r="Q55" s="93"/>
+      <c r="R55" s="93"/>
+      <c r="S55" s="93"/>
+      <c r="T55" s="93"/>
+      <c r="U55" s="93"/>
+      <c r="V55" s="93"/>
+      <c r="W55" s="93"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="94"/>
       <c r="AB55" s="56" t="s">
         <v>819</v>
       </c>
@@ -13063,7 +13075,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="58" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A58" s="54">
         <f t="shared" si="13"/>
         <v>40</v>
@@ -13175,36 +13187,36 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="59" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A59" s="54"/>
-      <c r="B59" s="111" t="s">
+      <c r="B59" s="92" t="s">
         <v>845</v>
       </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="112"/>
-      <c r="F59" s="112"/>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
-      <c r="M59" s="112"/>
-      <c r="N59" s="112"/>
-      <c r="O59" s="112"/>
-      <c r="P59" s="112"/>
-      <c r="Q59" s="112"/>
-      <c r="R59" s="112"/>
-      <c r="S59" s="112"/>
-      <c r="T59" s="112"/>
-      <c r="U59" s="112"/>
-      <c r="V59" s="112"/>
-      <c r="W59" s="112"/>
-      <c r="X59" s="112"/>
-      <c r="Y59" s="112"/>
-      <c r="Z59" s="112"/>
-      <c r="AA59" s="113"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="93"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="93"/>
+      <c r="J59" s="93"/>
+      <c r="K59" s="93"/>
+      <c r="L59" s="93"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="93"/>
+      <c r="O59" s="93"/>
+      <c r="P59" s="93"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="93"/>
+      <c r="T59" s="93"/>
+      <c r="U59" s="93"/>
+      <c r="V59" s="93"/>
+      <c r="W59" s="93"/>
+      <c r="X59" s="93"/>
+      <c r="Y59" s="93"/>
+      <c r="Z59" s="93"/>
+      <c r="AA59" s="94"/>
       <c r="AB59" s="56" t="s">
         <v>854</v>
       </c>
@@ -13528,85 +13540,78 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:80" ht="12" thickBot="1">
+    <row r="68" spans="1:80" ht="12.75" thickBot="1">
       <c r="A68" s="54"/>
       <c r="B68" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="C68" s="125" t="s">
+      <c r="C68" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="126"/>
-      <c r="E68" s="126"/>
-      <c r="F68" s="126"/>
-      <c r="G68" s="126"/>
-      <c r="H68" s="126"/>
-      <c r="I68" s="126"/>
-      <c r="J68" s="126"/>
-      <c r="K68" s="126"/>
-      <c r="L68" s="126"/>
-      <c r="M68" s="126"/>
-      <c r="N68" s="126"/>
-      <c r="O68" s="126"/>
-      <c r="P68" s="126"/>
-      <c r="Q68" s="126"/>
-      <c r="R68" s="126"/>
-      <c r="S68" s="126"/>
-      <c r="T68" s="126"/>
-      <c r="U68" s="126"/>
-      <c r="V68" s="126"/>
-      <c r="W68" s="126"/>
-      <c r="X68" s="126"/>
-      <c r="Y68" s="126"/>
-      <c r="Z68" s="126"/>
-      <c r="AA68" s="127"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="101"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="101"/>
+      <c r="O68" s="101"/>
+      <c r="P68" s="101"/>
+      <c r="Q68" s="101"/>
+      <c r="R68" s="101"/>
+      <c r="S68" s="101"/>
+      <c r="T68" s="101"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="101"/>
+      <c r="W68" s="101"/>
+      <c r="X68" s="101"/>
+      <c r="Y68" s="101"/>
+      <c r="Z68" s="101"/>
+      <c r="AA68" s="102"/>
       <c r="AB68" s="56"/>
     </row>
-    <row r="69" spans="1:80" ht="12" thickBot="1">
+    <row r="69" spans="1:80" ht="12.75" thickBot="1">
       <c r="B69" s="63"/>
-      <c r="C69" s="120"/>
-      <c r="D69" s="121"/>
-      <c r="E69" s="121"/>
-      <c r="F69" s="121"/>
-      <c r="G69" s="121"/>
-      <c r="H69" s="121"/>
-      <c r="I69" s="121"/>
-      <c r="J69" s="121"/>
-      <c r="K69" s="121"/>
-      <c r="L69" s="121"/>
-      <c r="M69" s="121"/>
-      <c r="N69" s="121"/>
-      <c r="O69" s="121"/>
-      <c r="P69" s="121"/>
-      <c r="Q69" s="121"/>
-      <c r="R69" s="121"/>
-      <c r="S69" s="121"/>
-      <c r="T69" s="121"/>
-      <c r="U69" s="121"/>
-      <c r="V69" s="121"/>
-      <c r="W69" s="121"/>
-      <c r="X69" s="121"/>
-      <c r="Y69" s="121"/>
-      <c r="Z69" s="121"/>
-      <c r="AA69" s="122"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="96"/>
+      <c r="F69" s="96"/>
+      <c r="G69" s="96"/>
+      <c r="H69" s="96"/>
+      <c r="I69" s="96"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="96"/>
+      <c r="M69" s="96"/>
+      <c r="N69" s="96"/>
+      <c r="O69" s="96"/>
+      <c r="P69" s="96"/>
+      <c r="Q69" s="96"/>
+      <c r="R69" s="96"/>
+      <c r="S69" s="96"/>
+      <c r="T69" s="96"/>
+      <c r="U69" s="96"/>
+      <c r="V69" s="96"/>
+      <c r="W69" s="96"/>
+      <c r="X69" s="96"/>
+      <c r="Y69" s="96"/>
+      <c r="Z69" s="96"/>
+      <c r="AA69" s="97"/>
       <c r="AB69" s="60"/>
       <c r="CB69" s="69"/>
     </row>
   </sheetData>
   <sheetProtection password="CC71" sheet="1" selectLockedCells="1"/>
   <mergeCells count="33">
-    <mergeCell ref="B59:AA59"/>
-    <mergeCell ref="B55:AA55"/>
-    <mergeCell ref="B48:AA48"/>
-    <mergeCell ref="C69:AA69"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="B33:AA33"/>
-    <mergeCell ref="C68:AA68"/>
-    <mergeCell ref="B52:AA52"/>
-    <mergeCell ref="B44:AA44"/>
-    <mergeCell ref="B36:AA36"/>
-    <mergeCell ref="B38:AA38"/>
-    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:W5"/>
     <mergeCell ref="C6:AA6"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="B9:AA9"/>
@@ -13623,11 +13628,18 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="W7:X7"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:W5"/>
+    <mergeCell ref="B59:AA59"/>
+    <mergeCell ref="B55:AA55"/>
+    <mergeCell ref="B48:AA48"/>
+    <mergeCell ref="C69:AA69"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="B33:AA33"/>
+    <mergeCell ref="C68:AA68"/>
+    <mergeCell ref="B52:AA52"/>
+    <mergeCell ref="B44:AA44"/>
+    <mergeCell ref="B36:AA36"/>
+    <mergeCell ref="B38:AA38"/>
+    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="C18:Z18">
@@ -14405,23 +14417,23 @@
       <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="11.65"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.3984375" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="23" width="3.86328125" style="26" customWidth="1"/>
-    <col min="24" max="24" width="4.59765625" style="26" customWidth="1"/>
-    <col min="25" max="25" width="5.59765625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="3.85546875" style="26" customWidth="1"/>
+    <col min="24" max="24" width="4.5703125" style="26" customWidth="1"/>
+    <col min="25" max="25" width="5.5703125" style="26" customWidth="1"/>
     <col min="26" max="26" width="5" style="26" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.86328125" style="26" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1328125" style="26" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="57.73046875" style="27" customWidth="1"/>
-    <col min="30" max="30" width="4.265625" style="74" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="26" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="57.7109375" style="27" customWidth="1"/>
+    <col min="30" max="30" width="4.28515625" style="74" bestFit="1" customWidth="1"/>
     <col min="31" max="61" width="3" style="74" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="6.59765625" style="27"/>
+    <col min="62" max="16384" width="6.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="12" thickBot="1">
+    <row r="1" spans="1:80" ht="12.75" thickBot="1">
       <c r="A1" s="23"/>
       <c r="B1" s="24"/>
       <c r="C1" s="25"/>
@@ -14547,7 +14559,7 @@
       </c>
     </row>
     <row r="2" spans="1:80" ht="12" customHeight="1" thickBot="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="115" t="s">
         <v>856</v>
       </c>
       <c r="B2" s="67" t="s">
@@ -14618,8 +14630,8 @@
         <v>781</v>
       </c>
     </row>
-    <row r="3" spans="1:80" ht="12" thickBot="1">
-      <c r="A3" s="93"/>
+    <row r="3" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A3" s="116"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34"/>
@@ -14648,15 +14660,15 @@
       <c r="AA3" s="36"/>
     </row>
     <row r="4" spans="1:80">
-      <c r="A4" s="93"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -14675,42 +14687,42 @@
       <c r="U4" s="37"/>
       <c r="V4" s="37"/>
       <c r="W4" s="38"/>
-      <c r="X4" s="97" t="s">
+      <c r="X4" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="98"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="121"/>
       <c r="AA4" s="39"/>
     </row>
-    <row r="5" spans="1:80" ht="12" thickBot="1">
-      <c r="A5" s="94"/>
+    <row r="5" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A5" s="117"/>
       <c r="B5" s="40"/>
-      <c r="C5" s="99" t="str">
+      <c r="C5" s="122" t="str">
         <f>IF(ISERROR((RIGHT(B5,LEN(B5)- FIND("_",B5)))),"",(RIGHT(B5,LEN(B5)- FIND("_",B5))))</f>
         <v/>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102" t="s">
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125" t="s">
         <v>807</v>
       </c>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="104"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="126"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="127"/>
       <c r="X5" s="72" t="s">
         <v>4</v>
       </c>
@@ -14722,7 +14734,7 @@
       </c>
       <c r="AA5" s="43"/>
     </row>
-    <row r="6" spans="1:80" ht="12" thickBot="1">
+    <row r="6" spans="1:80" ht="12.75" thickBot="1">
       <c r="A6" s="44"/>
       <c r="B6" s="45" t="s">
         <v>161</v>
@@ -14756,50 +14768,50 @@
       <c r="AA6" s="105"/>
     </row>
     <row r="7" spans="1:80" s="48" customFormat="1">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="106" t="s">
         <v>193</v>
       </c>
       <c r="D7" s="106"/>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="103" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="107" t="s">
+      <c r="F7" s="104"/>
+      <c r="G7" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="115"/>
-      <c r="I7" s="107" t="s">
+      <c r="H7" s="104"/>
+      <c r="I7" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="115"/>
-      <c r="K7" s="107" t="s">
+      <c r="J7" s="104"/>
+      <c r="K7" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="115"/>
-      <c r="M7" s="107" t="s">
+      <c r="L7" s="104"/>
+      <c r="M7" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="107" t="s">
+      <c r="N7" s="110"/>
+      <c r="O7" s="103" t="s">
         <v>199</v>
       </c>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="107" t="s">
+      <c r="P7" s="104"/>
+      <c r="Q7" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="114"/>
+      <c r="R7" s="110"/>
       <c r="S7" s="106" t="s">
         <v>201</v>
       </c>
       <c r="T7" s="106"/>
-      <c r="U7" s="107" t="s">
+      <c r="U7" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="V7" s="115"/>
+      <c r="V7" s="104"/>
       <c r="W7" s="106" t="s">
         <v>203</v>
       </c>
@@ -14807,8 +14819,8 @@
       <c r="Y7" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="123" t="s">
+      <c r="Z7" s="103"/>
+      <c r="AA7" s="98" t="s">
         <v>216</v>
       </c>
       <c r="AB7" s="46"/>
@@ -14865,9 +14877,9 @@
       <c r="CA7" s="47"/>
       <c r="CB7" s="47"/>
     </row>
-    <row r="8" spans="1:80" s="48" customFormat="1" ht="12" thickBot="1">
-      <c r="A8" s="118"/>
-      <c r="B8" s="119"/>
+    <row r="8" spans="1:80" s="48" customFormat="1" ht="12.75" thickBot="1">
+      <c r="A8" s="113"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="49" t="s">
         <v>0</v>
       </c>
@@ -14940,7 +14952,7 @@
       <c r="Z8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AA8" s="128"/>
+      <c r="AA8" s="130"/>
       <c r="AB8" s="46"/>
       <c r="AC8" s="27"/>
       <c r="AD8" s="74"/>
@@ -14995,38 +15007,38 @@
       <c r="CA8" s="47"/>
       <c r="CB8" s="47"/>
     </row>
-    <row r="9" spans="1:80" s="48" customFormat="1" ht="14.25" thickBot="1">
+    <row r="9" spans="1:80" s="48" customFormat="1" ht="15.75" thickBot="1">
       <c r="A9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="130"/>
-      <c r="D9" s="130"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="130"/>
-      <c r="P9" s="130"/>
-      <c r="Q9" s="130"/>
-      <c r="R9" s="130"/>
-      <c r="S9" s="130"/>
-      <c r="T9" s="130"/>
-      <c r="U9" s="130"/>
-      <c r="V9" s="130"/>
-      <c r="W9" s="130"/>
-      <c r="X9" s="130"/>
-      <c r="Y9" s="130"/>
-      <c r="Z9" s="130"/>
-      <c r="AA9" s="113"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="129"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="129"/>
+      <c r="O9" s="129"/>
+      <c r="P9" s="129"/>
+      <c r="Q9" s="129"/>
+      <c r="R9" s="129"/>
+      <c r="S9" s="129"/>
+      <c r="T9" s="129"/>
+      <c r="U9" s="129"/>
+      <c r="V9" s="129"/>
+      <c r="W9" s="129"/>
+      <c r="X9" s="129"/>
+      <c r="Y9" s="129"/>
+      <c r="Z9" s="129"/>
+      <c r="AA9" s="94"/>
       <c r="AB9" s="53" t="s">
         <v>207</v>
       </c>
@@ -15322,7 +15334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:80" ht="12" thickBot="1">
+    <row r="16" spans="1:80" ht="12.75" thickBot="1">
       <c r="A16" s="54">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -15362,36 +15374,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:61" s="59" customFormat="1" ht="14.25" thickBot="1">
+    <row r="17" spans="1:61" s="59" customFormat="1" ht="15.75" thickBot="1">
       <c r="A17" s="54"/>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="128" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="130"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="130"/>
-      <c r="F17" s="130"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="130"/>
-      <c r="I17" s="130"/>
-      <c r="J17" s="130"/>
-      <c r="K17" s="130"/>
-      <c r="L17" s="130"/>
-      <c r="M17" s="130"/>
-      <c r="N17" s="130"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="130"/>
-      <c r="Q17" s="130"/>
-      <c r="R17" s="130"/>
-      <c r="S17" s="130"/>
-      <c r="T17" s="130"/>
-      <c r="U17" s="130"/>
-      <c r="V17" s="130"/>
-      <c r="W17" s="130"/>
-      <c r="X17" s="130"/>
-      <c r="Y17" s="130"/>
-      <c r="Z17" s="130"/>
-      <c r="AA17" s="113"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="129"/>
+      <c r="K17" s="129"/>
+      <c r="L17" s="129"/>
+      <c r="M17" s="129"/>
+      <c r="N17" s="129"/>
+      <c r="O17" s="129"/>
+      <c r="P17" s="129"/>
+      <c r="Q17" s="129"/>
+      <c r="R17" s="129"/>
+      <c r="S17" s="129"/>
+      <c r="T17" s="129"/>
+      <c r="U17" s="129"/>
+      <c r="V17" s="129"/>
+      <c r="W17" s="129"/>
+      <c r="X17" s="129"/>
+      <c r="Y17" s="129"/>
+      <c r="Z17" s="129"/>
+      <c r="AA17" s="94"/>
       <c r="AB17" s="58" t="s">
         <v>18</v>
       </c>
@@ -15541,7 +15553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:61" ht="12" thickBot="1">
+    <row r="20" spans="1:61" ht="12.75" thickBot="1">
       <c r="A20" s="54">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -15581,36 +15593,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:61" ht="14.25" thickBot="1">
+    <row r="21" spans="1:61" ht="15.75" thickBot="1">
       <c r="A21" s="54"/>
-      <c r="B21" s="129" t="s">
+      <c r="B21" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="130"/>
-      <c r="D21" s="130"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="130"/>
-      <c r="I21" s="130"/>
-      <c r="J21" s="130"/>
-      <c r="K21" s="130"/>
-      <c r="L21" s="130"/>
-      <c r="M21" s="130"/>
-      <c r="N21" s="130"/>
-      <c r="O21" s="130"/>
-      <c r="P21" s="130"/>
-      <c r="Q21" s="130"/>
-      <c r="R21" s="130"/>
-      <c r="S21" s="130"/>
-      <c r="T21" s="130"/>
-      <c r="U21" s="130"/>
-      <c r="V21" s="130"/>
-      <c r="W21" s="130"/>
-      <c r="X21" s="130"/>
-      <c r="Y21" s="130"/>
-      <c r="Z21" s="130"/>
-      <c r="AA21" s="113"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
+      <c r="J21" s="129"/>
+      <c r="K21" s="129"/>
+      <c r="L21" s="129"/>
+      <c r="M21" s="129"/>
+      <c r="N21" s="129"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="129"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
+      <c r="S21" s="129"/>
+      <c r="T21" s="129"/>
+      <c r="U21" s="129"/>
+      <c r="V21" s="129"/>
+      <c r="W21" s="129"/>
+      <c r="X21" s="129"/>
+      <c r="Y21" s="129"/>
+      <c r="Z21" s="129"/>
+      <c r="AA21" s="94"/>
       <c r="AB21" s="60" t="s">
         <v>17</v>
       </c>
@@ -16014,7 +16026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:61" ht="12" thickBot="1">
+    <row r="32" spans="1:61" ht="12.75" thickBot="1">
       <c r="A32" s="54">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -16054,36 +16066,36 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:61" ht="14.25" thickBot="1">
+    <row r="33" spans="1:61" ht="15.75" thickBot="1">
       <c r="A33" s="54"/>
-      <c r="B33" s="129" t="s">
+      <c r="B33" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="130"/>
-      <c r="D33" s="130"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="130"/>
-      <c r="I33" s="130"/>
-      <c r="J33" s="130"/>
-      <c r="K33" s="130"/>
-      <c r="L33" s="130"/>
-      <c r="M33" s="130"/>
-      <c r="N33" s="130"/>
-      <c r="O33" s="130"/>
-      <c r="P33" s="130"/>
-      <c r="Q33" s="130"/>
-      <c r="R33" s="130"/>
-      <c r="S33" s="130"/>
-      <c r="T33" s="130"/>
-      <c r="U33" s="130"/>
-      <c r="V33" s="130"/>
-      <c r="W33" s="130"/>
-      <c r="X33" s="130"/>
-      <c r="Y33" s="130"/>
-      <c r="Z33" s="130"/>
-      <c r="AA33" s="113"/>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="129"/>
+      <c r="J33" s="129"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
+      <c r="O33" s="129"/>
+      <c r="P33" s="129"/>
+      <c r="Q33" s="129"/>
+      <c r="R33" s="129"/>
+      <c r="S33" s="129"/>
+      <c r="T33" s="129"/>
+      <c r="U33" s="129"/>
+      <c r="V33" s="129"/>
+      <c r="W33" s="129"/>
+      <c r="X33" s="129"/>
+      <c r="Y33" s="129"/>
+      <c r="Z33" s="129"/>
+      <c r="AA33" s="94"/>
       <c r="AB33" s="60" t="s">
         <v>15</v>
       </c>
@@ -16127,7 +16139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:61" ht="12" thickBot="1">
+    <row r="35" spans="1:61" ht="12.75" thickBot="1">
       <c r="A35" s="54">
         <f t="shared" ref="A35" si="5">IF(ISERROR((A34+1)),"",(A34+1))</f>
         <v>23</v>
@@ -16167,41 +16179,41 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:61" ht="14.25" thickBot="1">
+    <row r="36" spans="1:61" ht="15.75" thickBot="1">
       <c r="A36" s="54"/>
-      <c r="B36" s="129" t="s">
+      <c r="B36" s="128" t="s">
         <v>757</v>
       </c>
-      <c r="C36" s="130"/>
-      <c r="D36" s="130"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="130"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="130"/>
-      <c r="I36" s="130"/>
-      <c r="J36" s="130"/>
-      <c r="K36" s="130"/>
-      <c r="L36" s="130"/>
-      <c r="M36" s="130"/>
-      <c r="N36" s="130"/>
-      <c r="O36" s="130"/>
-      <c r="P36" s="130"/>
-      <c r="Q36" s="130"/>
-      <c r="R36" s="130"/>
-      <c r="S36" s="130"/>
-      <c r="T36" s="130"/>
-      <c r="U36" s="130"/>
-      <c r="V36" s="130"/>
-      <c r="W36" s="130"/>
-      <c r="X36" s="130"/>
-      <c r="Y36" s="130"/>
-      <c r="Z36" s="130"/>
-      <c r="AA36" s="113"/>
+      <c r="C36" s="129"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="129"/>
+      <c r="K36" s="129"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="129"/>
+      <c r="N36" s="129"/>
+      <c r="O36" s="129"/>
+      <c r="P36" s="129"/>
+      <c r="Q36" s="129"/>
+      <c r="R36" s="129"/>
+      <c r="S36" s="129"/>
+      <c r="T36" s="129"/>
+      <c r="U36" s="129"/>
+      <c r="V36" s="129"/>
+      <c r="W36" s="129"/>
+      <c r="X36" s="129"/>
+      <c r="Y36" s="129"/>
+      <c r="Z36" s="129"/>
+      <c r="AA36" s="94"/>
       <c r="AB36" s="56" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="37" spans="1:61" ht="12" thickBot="1">
+    <row r="37" spans="1:61" ht="12.75" thickBot="1">
       <c r="A37" s="54">
         <v>24</v>
       </c>
@@ -16240,36 +16252,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:61" ht="14.25" thickBot="1">
+    <row r="38" spans="1:61" ht="15.75" thickBot="1">
       <c r="A38" s="54"/>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="128" t="s">
         <v>761</v>
       </c>
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="130"/>
-      <c r="I38" s="130"/>
-      <c r="J38" s="130"/>
-      <c r="K38" s="130"/>
-      <c r="L38" s="130"/>
-      <c r="M38" s="130"/>
-      <c r="N38" s="130"/>
-      <c r="O38" s="130"/>
-      <c r="P38" s="130"/>
-      <c r="Q38" s="130"/>
-      <c r="R38" s="130"/>
-      <c r="S38" s="130"/>
-      <c r="T38" s="130"/>
-      <c r="U38" s="130"/>
-      <c r="V38" s="130"/>
-      <c r="W38" s="130"/>
-      <c r="X38" s="130"/>
-      <c r="Y38" s="130"/>
-      <c r="Z38" s="130"/>
-      <c r="AA38" s="113"/>
+      <c r="C38" s="129"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="129"/>
+      <c r="F38" s="129"/>
+      <c r="G38" s="129"/>
+      <c r="H38" s="129"/>
+      <c r="I38" s="129"/>
+      <c r="J38" s="129"/>
+      <c r="K38" s="129"/>
+      <c r="L38" s="129"/>
+      <c r="M38" s="129"/>
+      <c r="N38" s="129"/>
+      <c r="O38" s="129"/>
+      <c r="P38" s="129"/>
+      <c r="Q38" s="129"/>
+      <c r="R38" s="129"/>
+      <c r="S38" s="129"/>
+      <c r="T38" s="129"/>
+      <c r="U38" s="129"/>
+      <c r="V38" s="129"/>
+      <c r="W38" s="129"/>
+      <c r="X38" s="129"/>
+      <c r="Y38" s="129"/>
+      <c r="Z38" s="129"/>
+      <c r="AA38" s="94"/>
       <c r="AB38" s="56" t="s">
         <v>0</v>
       </c>
@@ -16433,7 +16445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:61" ht="12" thickBot="1">
+    <row r="43" spans="1:61" ht="12.75" thickBot="1">
       <c r="A43" s="54">
         <v>29</v>
       </c>
@@ -16472,36 +16484,36 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:61" ht="14.25" thickBot="1">
+    <row r="44" spans="1:61" ht="15.75" thickBot="1">
       <c r="A44" s="54"/>
-      <c r="B44" s="111" t="s">
+      <c r="B44" s="92" t="s">
         <v>801</v>
       </c>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="112"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
-      <c r="K44" s="112"/>
-      <c r="L44" s="112"/>
-      <c r="M44" s="112"/>
-      <c r="N44" s="112"/>
-      <c r="O44" s="112"/>
-      <c r="P44" s="112"/>
-      <c r="Q44" s="112"/>
-      <c r="R44" s="112"/>
-      <c r="S44" s="112"/>
-      <c r="T44" s="112"/>
-      <c r="U44" s="112"/>
-      <c r="V44" s="112"/>
-      <c r="W44" s="112"/>
-      <c r="X44" s="112"/>
-      <c r="Y44" s="112"/>
-      <c r="Z44" s="112"/>
-      <c r="AA44" s="113"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="94"/>
       <c r="AB44" s="56" t="s">
         <v>802</v>
       </c>
@@ -16584,7 +16596,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:61" ht="12" thickBot="1">
+    <row r="47" spans="1:61" ht="12.75" thickBot="1">
       <c r="A47" s="54">
         <v>32</v>
       </c>
@@ -16623,36 +16635,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:61" ht="14.25" thickBot="1">
+    <row r="48" spans="1:61" ht="15.75" thickBot="1">
       <c r="A48" s="54"/>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="92" t="s">
         <v>810</v>
       </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="M48" s="112"/>
-      <c r="N48" s="112"/>
-      <c r="O48" s="112"/>
-      <c r="P48" s="112"/>
-      <c r="Q48" s="112"/>
-      <c r="R48" s="112"/>
-      <c r="S48" s="112"/>
-      <c r="T48" s="112"/>
-      <c r="U48" s="112"/>
-      <c r="V48" s="112"/>
-      <c r="W48" s="112"/>
-      <c r="X48" s="112"/>
-      <c r="Y48" s="112"/>
-      <c r="Z48" s="112"/>
-      <c r="AA48" s="113"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="93"/>
+      <c r="P48" s="93"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="93"/>
+      <c r="T48" s="93"/>
+      <c r="U48" s="93"/>
+      <c r="V48" s="93"/>
+      <c r="W48" s="93"/>
+      <c r="X48" s="93"/>
+      <c r="Y48" s="93"/>
+      <c r="Z48" s="93"/>
+      <c r="AA48" s="94"/>
       <c r="AB48" s="56" t="s">
         <v>814</v>
       </c>
@@ -16831,7 +16843,7 @@
       <c r="BH50" s="27"/>
       <c r="BI50" s="27"/>
     </row>
-    <row r="51" spans="1:61" ht="12" thickBot="1">
+    <row r="51" spans="1:61" ht="12.75" thickBot="1">
       <c r="A51" s="54">
         <v>35</v>
       </c>
@@ -16902,36 +16914,36 @@
       <c r="BH51" s="27"/>
       <c r="BI51" s="27"/>
     </row>
-    <row r="52" spans="1:61" ht="14.25" thickBot="1">
+    <row r="52" spans="1:61" ht="15.75" thickBot="1">
       <c r="A52" s="54"/>
-      <c r="B52" s="111" t="s">
+      <c r="B52" s="92" t="s">
         <v>821</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="112"/>
-      <c r="L52" s="112"/>
-      <c r="M52" s="112"/>
-      <c r="N52" s="112"/>
-      <c r="O52" s="112"/>
-      <c r="P52" s="112"/>
-      <c r="Q52" s="112"/>
-      <c r="R52" s="112"/>
-      <c r="S52" s="112"/>
-      <c r="T52" s="112"/>
-      <c r="U52" s="112"/>
-      <c r="V52" s="112"/>
-      <c r="W52" s="112"/>
-      <c r="X52" s="112"/>
-      <c r="Y52" s="112"/>
-      <c r="Z52" s="112"/>
-      <c r="AA52" s="113"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
+      <c r="K52" s="93"/>
+      <c r="L52" s="93"/>
+      <c r="M52" s="93"/>
+      <c r="N52" s="93"/>
+      <c r="O52" s="93"/>
+      <c r="P52" s="93"/>
+      <c r="Q52" s="93"/>
+      <c r="R52" s="93"/>
+      <c r="S52" s="93"/>
+      <c r="T52" s="93"/>
+      <c r="U52" s="93"/>
+      <c r="V52" s="93"/>
+      <c r="W52" s="93"/>
+      <c r="X52" s="93"/>
+      <c r="Y52" s="93"/>
+      <c r="Z52" s="93"/>
+      <c r="AA52" s="94"/>
       <c r="AB52" s="56" t="s">
         <v>820</v>
       </c>
@@ -17110,36 +17122,36 @@
       <c r="BH54" s="27"/>
       <c r="BI54" s="27"/>
     </row>
-    <row r="55" spans="1:61" ht="14.25" hidden="1" thickBot="1">
+    <row r="55" spans="1:61" ht="15.75" hidden="1" thickBot="1">
       <c r="A55" s="54"/>
-      <c r="B55" s="111" t="s">
+      <c r="B55" s="92" t="s">
         <v>818</v>
       </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="112"/>
-      <c r="L55" s="112"/>
-      <c r="M55" s="112"/>
-      <c r="N55" s="112"/>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
-      <c r="Q55" s="112"/>
-      <c r="R55" s="112"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="112"/>
-      <c r="U55" s="112"/>
-      <c r="V55" s="112"/>
-      <c r="W55" s="112"/>
-      <c r="X55" s="112"/>
-      <c r="Y55" s="112"/>
-      <c r="Z55" s="112"/>
-      <c r="AA55" s="113"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="93"/>
+      <c r="J55" s="93"/>
+      <c r="K55" s="93"/>
+      <c r="L55" s="93"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="93"/>
+      <c r="O55" s="93"/>
+      <c r="P55" s="93"/>
+      <c r="Q55" s="93"/>
+      <c r="R55" s="93"/>
+      <c r="S55" s="93"/>
+      <c r="T55" s="93"/>
+      <c r="U55" s="93"/>
+      <c r="V55" s="93"/>
+      <c r="W55" s="93"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="94"/>
       <c r="AB55" s="56" t="s">
         <v>819</v>
       </c>
@@ -17319,7 +17331,7 @@
       <c r="BH57" s="27"/>
       <c r="BI57" s="27"/>
     </row>
-    <row r="58" spans="1:61" ht="12" hidden="1" thickBot="1">
+    <row r="58" spans="1:61" ht="12.75" hidden="1" thickBot="1">
       <c r="A58" s="54">
         <f t="shared" si="13"/>
         <v>40</v>
@@ -17463,36 +17475,36 @@
       <c r="BH58" s="27"/>
       <c r="BI58" s="27"/>
     </row>
-    <row r="59" spans="1:61" ht="14.25" hidden="1" thickBot="1">
+    <row r="59" spans="1:61" ht="15.75" hidden="1" thickBot="1">
       <c r="A59" s="54"/>
-      <c r="B59" s="111" t="s">
+      <c r="B59" s="92" t="s">
         <v>845</v>
       </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="112"/>
-      <c r="F59" s="112"/>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
-      <c r="M59" s="112"/>
-      <c r="N59" s="112"/>
-      <c r="O59" s="112"/>
-      <c r="P59" s="112"/>
-      <c r="Q59" s="112"/>
-      <c r="R59" s="112"/>
-      <c r="S59" s="112"/>
-      <c r="T59" s="112"/>
-      <c r="U59" s="112"/>
-      <c r="V59" s="112"/>
-      <c r="W59" s="112"/>
-      <c r="X59" s="112"/>
-      <c r="Y59" s="112"/>
-      <c r="Z59" s="112"/>
-      <c r="AA59" s="113"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="93"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="93"/>
+      <c r="J59" s="93"/>
+      <c r="K59" s="93"/>
+      <c r="L59" s="93"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="93"/>
+      <c r="O59" s="93"/>
+      <c r="P59" s="93"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="93"/>
+      <c r="T59" s="93"/>
+      <c r="U59" s="93"/>
+      <c r="V59" s="93"/>
+      <c r="W59" s="93"/>
+      <c r="X59" s="93"/>
+      <c r="Y59" s="93"/>
+      <c r="Z59" s="93"/>
+      <c r="AA59" s="94"/>
       <c r="AB59" s="56" t="s">
         <v>854</v>
       </c>
@@ -18104,38 +18116,38 @@
       <c r="BH67" s="27"/>
       <c r="BI67" s="27"/>
     </row>
-    <row r="68" spans="1:80" ht="12" thickBot="1">
+    <row r="68" spans="1:80" ht="12.75" thickBot="1">
       <c r="A68" s="54"/>
       <c r="B68" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="C68" s="125" t="s">
+      <c r="C68" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="126"/>
-      <c r="E68" s="126"/>
-      <c r="F68" s="126"/>
-      <c r="G68" s="126"/>
-      <c r="H68" s="126"/>
-      <c r="I68" s="126"/>
-      <c r="J68" s="126"/>
-      <c r="K68" s="126"/>
-      <c r="L68" s="126"/>
-      <c r="M68" s="126"/>
-      <c r="N68" s="126"/>
-      <c r="O68" s="126"/>
-      <c r="P68" s="126"/>
-      <c r="Q68" s="126"/>
-      <c r="R68" s="126"/>
-      <c r="S68" s="126"/>
-      <c r="T68" s="126"/>
-      <c r="U68" s="126"/>
-      <c r="V68" s="126"/>
-      <c r="W68" s="126"/>
-      <c r="X68" s="126"/>
-      <c r="Y68" s="126"/>
-      <c r="Z68" s="126"/>
-      <c r="AA68" s="127"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="101"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="101"/>
+      <c r="O68" s="101"/>
+      <c r="P68" s="101"/>
+      <c r="Q68" s="101"/>
+      <c r="R68" s="101"/>
+      <c r="S68" s="101"/>
+      <c r="T68" s="101"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="101"/>
+      <c r="W68" s="101"/>
+      <c r="X68" s="101"/>
+      <c r="Y68" s="101"/>
+      <c r="Z68" s="101"/>
+      <c r="AA68" s="102"/>
       <c r="AB68" s="56"/>
       <c r="AD68" s="27"/>
       <c r="AE68" s="27"/>
@@ -18170,33 +18182,33 @@
       <c r="BH68" s="27"/>
       <c r="BI68" s="27"/>
     </row>
-    <row r="69" spans="1:80" ht="12" thickBot="1">
+    <row r="69" spans="1:80" ht="12.75" thickBot="1">
       <c r="B69" s="63"/>
-      <c r="C69" s="120"/>
-      <c r="D69" s="121"/>
-      <c r="E69" s="121"/>
-      <c r="F69" s="121"/>
-      <c r="G69" s="121"/>
-      <c r="H69" s="121"/>
-      <c r="I69" s="121"/>
-      <c r="J69" s="121"/>
-      <c r="K69" s="121"/>
-      <c r="L69" s="121"/>
-      <c r="M69" s="121"/>
-      <c r="N69" s="121"/>
-      <c r="O69" s="121"/>
-      <c r="P69" s="121"/>
-      <c r="Q69" s="121"/>
-      <c r="R69" s="121"/>
-      <c r="S69" s="121"/>
-      <c r="T69" s="121"/>
-      <c r="U69" s="121"/>
-      <c r="V69" s="121"/>
-      <c r="W69" s="121"/>
-      <c r="X69" s="121"/>
-      <c r="Y69" s="121"/>
-      <c r="Z69" s="121"/>
-      <c r="AA69" s="122"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="96"/>
+      <c r="F69" s="96"/>
+      <c r="G69" s="96"/>
+      <c r="H69" s="96"/>
+      <c r="I69" s="96"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="96"/>
+      <c r="M69" s="96"/>
+      <c r="N69" s="96"/>
+      <c r="O69" s="96"/>
+      <c r="P69" s="96"/>
+      <c r="Q69" s="96"/>
+      <c r="R69" s="96"/>
+      <c r="S69" s="96"/>
+      <c r="T69" s="96"/>
+      <c r="U69" s="96"/>
+      <c r="V69" s="96"/>
+      <c r="W69" s="96"/>
+      <c r="X69" s="96"/>
+      <c r="Y69" s="96"/>
+      <c r="Z69" s="96"/>
+      <c r="AA69" s="97"/>
       <c r="AB69" s="60"/>
       <c r="AD69" s="27"/>
       <c r="AE69" s="27"/>
@@ -18235,29 +18247,6 @@
   </sheetData>
   <sheetProtection password="CC71" sheet="1" selectLockedCells="1"/>
   <mergeCells count="33">
-    <mergeCell ref="B9:AA9"/>
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="B21:AA21"/>
-    <mergeCell ref="B33:AA33"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="B55:AA55"/>
-    <mergeCell ref="C68:AA68"/>
-    <mergeCell ref="C69:AA69"/>
-    <mergeCell ref="B44:AA44"/>
-    <mergeCell ref="B36:AA36"/>
-    <mergeCell ref="B38:AA38"/>
-    <mergeCell ref="B59:AA59"/>
-    <mergeCell ref="B52:AA52"/>
-    <mergeCell ref="B48:AA48"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:W5"/>
     <mergeCell ref="C6:AA6"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="C7:D7"/>
@@ -18268,6 +18257,29 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:W5"/>
+    <mergeCell ref="B55:AA55"/>
+    <mergeCell ref="C68:AA68"/>
+    <mergeCell ref="C69:AA69"/>
+    <mergeCell ref="B44:AA44"/>
+    <mergeCell ref="B36:AA36"/>
+    <mergeCell ref="B38:AA38"/>
+    <mergeCell ref="B59:AA59"/>
+    <mergeCell ref="B52:AA52"/>
+    <mergeCell ref="B48:AA48"/>
+    <mergeCell ref="B9:AA9"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="B21:AA21"/>
+    <mergeCell ref="B33:AA33"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:Z18">
     <cfRule type="notContainsBlanks" dxfId="317" priority="262">
@@ -19216,31 +19228,31 @@
   </sheetPr>
   <dimension ref="A1:CB69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="71" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="71" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Y45" sqref="Y45"/>
       <selection pane="topRight" activeCell="Y45" sqref="Y45"/>
       <selection pane="bottomLeft" activeCell="Y45" sqref="Y45"/>
-      <selection pane="bottomRight" activeCell="Z60" sqref="Z60"/>
+      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="11.65"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.3984375" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="23" width="3.86328125" style="26" customWidth="1"/>
-    <col min="24" max="24" width="5.1328125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.85546875" style="64" customWidth="1"/>
+    <col min="3" max="23" width="3.85546875" style="26" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" style="26" customWidth="1"/>
     <col min="25" max="25" width="5" style="26" customWidth="1"/>
-    <col min="26" max="26" width="6.265625" style="26" customWidth="1"/>
-    <col min="27" max="27" width="4.265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" style="26" customWidth="1"/>
+    <col min="27" max="27" width="4.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="26" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="57.73046875" style="27" customWidth="1"/>
-    <col min="30" max="30" width="4.3984375" style="27" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="57.7109375" style="27" customWidth="1"/>
+    <col min="30" max="30" width="4.42578125" style="27" bestFit="1" customWidth="1"/>
     <col min="31" max="61" width="3" style="27" bestFit="1" customWidth="1"/>
-    <col min="62" max="16384" width="6.59765625" style="27"/>
+    <col min="62" max="16384" width="6.5703125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="12" thickBot="1">
+    <row r="1" spans="1:80" ht="12.75" thickBot="1">
       <c r="A1" s="23"/>
       <c r="B1" s="24"/>
       <c r="C1" s="25"/>
@@ -19365,8 +19377,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="2" spans="1:80" ht="12" thickBot="1">
-      <c r="A2" s="92" t="s">
+    <row r="2" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A2" s="115" t="s">
         <v>856</v>
       </c>
       <c r="B2" s="67" t="s">
@@ -19456,8 +19468,8 @@
       <c r="BH2" s="74"/>
       <c r="BI2" s="74"/>
     </row>
-    <row r="3" spans="1:80" ht="12" thickBot="1">
-      <c r="A3" s="93"/>
+    <row r="3" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A3" s="116"/>
       <c r="B3" s="32"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34"/>
@@ -19486,15 +19498,15 @@
       <c r="AA3" s="36"/>
     </row>
     <row r="4" spans="1:80">
-      <c r="A4" s="93"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -19513,42 +19525,42 @@
       <c r="U4" s="37"/>
       <c r="V4" s="37"/>
       <c r="W4" s="38"/>
-      <c r="X4" s="97" t="s">
+      <c r="X4" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="98"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="121"/>
       <c r="AA4" s="39"/>
     </row>
-    <row r="5" spans="1:80" ht="12" thickBot="1">
-      <c r="A5" s="94"/>
+    <row r="5" spans="1:80" ht="12.75" thickBot="1">
+      <c r="A5" s="117"/>
       <c r="B5" s="40"/>
-      <c r="C5" s="99" t="str">
+      <c r="C5" s="122" t="str">
         <f>IF(ISERROR((RIGHT(B5,LEN(B5)- FIND("_",B5)))),"",(RIGHT(B5,LEN(B5)- FIND("_",B5))))</f>
         <v/>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102" t="s">
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125" t="s">
         <v>807</v>
       </c>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="104"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="126"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="127"/>
       <c r="X5" s="41" t="s">
         <v>4</v>
       </c>
@@ -19560,7 +19572,7 @@
       </c>
       <c r="AA5" s="43"/>
     </row>
-    <row r="6" spans="1:80" ht="12" thickBot="1">
+    <row r="6" spans="1:80" ht="12.75" thickBot="1">
       <c r="A6" s="44"/>
       <c r="B6" s="45" t="s">
         <v>161</v>
@@ -19594,50 +19606,50 @@
       <c r="AA6" s="105"/>
     </row>
     <row r="7" spans="1:80" s="48" customFormat="1">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="106" t="s">
         <v>193</v>
       </c>
       <c r="D7" s="106"/>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="103" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="107" t="s">
+      <c r="F7" s="104"/>
+      <c r="G7" s="103" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="115"/>
-      <c r="I7" s="107" t="s">
+      <c r="H7" s="104"/>
+      <c r="I7" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="115"/>
-      <c r="K7" s="107" t="s">
+      <c r="J7" s="104"/>
+      <c r="K7" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="115"/>
-      <c r="M7" s="107" t="s">
+      <c r="L7" s="104"/>
+      <c r="M7" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="107" t="s">
+      <c r="N7" s="110"/>
+      <c r="O7" s="103" t="s">
         <v>199</v>
       </c>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="107" t="s">
+      <c r="P7" s="104"/>
+      <c r="Q7" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="R7" s="114"/>
+      <c r="R7" s="110"/>
       <c r="S7" s="106" t="s">
         <v>201</v>
       </c>
       <c r="T7" s="106"/>
-      <c r="U7" s="107" t="s">
+      <c r="U7" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="V7" s="115"/>
+      <c r="V7" s="104"/>
       <c r="W7" s="106" t="s">
         <v>203</v>
       </c>
@@ -19645,8 +19657,8 @@
       <c r="Y7" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="123" t="s">
+      <c r="Z7" s="103"/>
+      <c r="AA7" s="98" t="s">
         <v>216</v>
       </c>
       <c r="AB7" s="46"/>
@@ -19703,9 +19715,9 @@
       <c r="CA7" s="47"/>
       <c r="CB7" s="47"/>
     </row>
-    <row r="8" spans="1:80" s="48" customFormat="1" ht="12" thickBot="1">
-      <c r="A8" s="118"/>
-      <c r="B8" s="119"/>
+    <row r="8" spans="1:80" s="48" customFormat="1" ht="12.75" thickBot="1">
+      <c r="A8" s="113"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="49" t="s">
         <v>0</v>
       </c>
@@ -19778,7 +19790,7 @@
       <c r="Z8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="AA8" s="124"/>
+      <c r="AA8" s="99"/>
       <c r="AB8" s="46"/>
       <c r="AC8" s="27"/>
       <c r="AD8" s="47"/>
@@ -19833,38 +19845,38 @@
       <c r="CA8" s="47"/>
       <c r="CB8" s="47"/>
     </row>
-    <row r="9" spans="1:80" s="48" customFormat="1" ht="14.25" hidden="1" thickBot="1">
+    <row r="9" spans="1:80" s="48" customFormat="1" ht="15.75" hidden="1" thickBot="1">
       <c r="A9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="109"/>
-      <c r="Q9" s="109"/>
-      <c r="R9" s="109"/>
-      <c r="S9" s="109"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="109"/>
-      <c r="V9" s="109"/>
-      <c r="W9" s="109"/>
-      <c r="X9" s="109"/>
-      <c r="Y9" s="109"/>
-      <c r="Z9" s="109"/>
-      <c r="AA9" s="110"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="J9" s="108"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108"/>
+      <c r="U9" s="108"/>
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="108"/>
+      <c r="Y9" s="108"/>
+      <c r="Z9" s="108"/>
+      <c r="AA9" s="109"/>
       <c r="AB9" s="53" t="s">
         <v>207</v>
       </c>
@@ -20160,7 +20172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:80" ht="12" hidden="1" thickBot="1">
+    <row r="16" spans="1:80" ht="12.75" hidden="1" thickBot="1">
       <c r="A16" s="54">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -20200,36 +20212,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="59" customFormat="1" ht="14.25" hidden="1" thickBot="1">
+    <row r="17" spans="1:29" s="59" customFormat="1" ht="15.75" hidden="1" thickBot="1">
       <c r="A17" s="54"/>
-      <c r="B17" s="111" t="s">
+      <c r="B17" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="112"/>
-      <c r="N17" s="112"/>
-      <c r="O17" s="112"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
-      <c r="V17" s="112"/>
-      <c r="W17" s="112"/>
-      <c r="X17" s="112"/>
-      <c r="Y17" s="112"/>
-      <c r="Z17" s="112"/>
-      <c r="AA17" s="113"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="93"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="93"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17" s="93"/>
+      <c r="R17" s="93"/>
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="93"/>
+      <c r="V17" s="93"/>
+      <c r="W17" s="93"/>
+      <c r="X17" s="93"/>
+      <c r="Y17" s="93"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="94"/>
       <c r="AB17" s="58" t="s">
         <v>18</v>
       </c>
@@ -20315,7 +20327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="12" hidden="1" thickBot="1">
+    <row r="20" spans="1:29" ht="12.75" hidden="1" thickBot="1">
       <c r="A20" s="54">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -20355,36 +20367,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="14.25" hidden="1" thickBot="1">
+    <row r="21" spans="1:29" ht="15.75" hidden="1" thickBot="1">
       <c r="A21" s="54"/>
-      <c r="B21" s="111" t="s">
+      <c r="B21" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
-      <c r="N21" s="112"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="112"/>
-      <c r="Q21" s="112"/>
-      <c r="R21" s="112"/>
-      <c r="S21" s="112"/>
-      <c r="T21" s="112"/>
-      <c r="U21" s="112"/>
-      <c r="V21" s="112"/>
-      <c r="W21" s="112"/>
-      <c r="X21" s="112"/>
-      <c r="Y21" s="112"/>
-      <c r="Z21" s="112"/>
-      <c r="AA21" s="113"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="93"/>
+      <c r="O21" s="93"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="93"/>
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="93"/>
+      <c r="W21" s="93"/>
+      <c r="X21" s="93"/>
+      <c r="Y21" s="93"/>
+      <c r="Z21" s="93"/>
+      <c r="AA21" s="94"/>
       <c r="AB21" s="60" t="s">
         <v>17</v>
       </c>
@@ -20788,7 +20800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="12" hidden="1" thickBot="1">
+    <row r="32" spans="1:29" ht="12.75" hidden="1" thickBot="1">
       <c r="A32" s="54">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -20828,36 +20840,36 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="33" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A33" s="54"/>
-      <c r="B33" s="111" t="s">
+      <c r="B33" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="112"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
-      <c r="K33" s="112"/>
-      <c r="L33" s="112"/>
-      <c r="M33" s="112"/>
-      <c r="N33" s="112"/>
-      <c r="O33" s="112"/>
-      <c r="P33" s="112"/>
-      <c r="Q33" s="112"/>
-      <c r="R33" s="112"/>
-      <c r="S33" s="112"/>
-      <c r="T33" s="112"/>
-      <c r="U33" s="112"/>
-      <c r="V33" s="112"/>
-      <c r="W33" s="112"/>
-      <c r="X33" s="112"/>
-      <c r="Y33" s="112"/>
-      <c r="Z33" s="112"/>
-      <c r="AA33" s="113"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="93"/>
+      <c r="V33" s="93"/>
+      <c r="W33" s="93"/>
+      <c r="X33" s="93"/>
+      <c r="Y33" s="93"/>
+      <c r="Z33" s="93"/>
+      <c r="AA33" s="94"/>
       <c r="AB33" s="60" t="s">
         <v>15</v>
       </c>
@@ -20901,7 +20913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="35" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A35" s="54">
         <f t="shared" ref="A35" si="4">IF(ISERROR((A34+1)),"",(A34+1))</f>
         <v>23</v>
@@ -20941,36 +20953,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="36" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A36" s="54"/>
-      <c r="B36" s="111" t="s">
+      <c r="B36" s="92" t="s">
         <v>757</v>
       </c>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="112"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="112"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="112"/>
-      <c r="M36" s="112"/>
-      <c r="N36" s="112"/>
-      <c r="O36" s="112"/>
-      <c r="P36" s="112"/>
-      <c r="Q36" s="112"/>
-      <c r="R36" s="112"/>
-      <c r="S36" s="112"/>
-      <c r="T36" s="112"/>
-      <c r="U36" s="112"/>
-      <c r="V36" s="112"/>
-      <c r="W36" s="112"/>
-      <c r="X36" s="112"/>
-      <c r="Y36" s="112"/>
-      <c r="Z36" s="112"/>
-      <c r="AA36" s="113"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="93"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="93"/>
+      <c r="O36" s="93"/>
+      <c r="P36" s="93"/>
+      <c r="Q36" s="93"/>
+      <c r="R36" s="93"/>
+      <c r="S36" s="93"/>
+      <c r="T36" s="93"/>
+      <c r="U36" s="93"/>
+      <c r="V36" s="93"/>
+      <c r="W36" s="93"/>
+      <c r="X36" s="93"/>
+      <c r="Y36" s="93"/>
+      <c r="Z36" s="93"/>
+      <c r="AA36" s="94"/>
       <c r="AB36" s="56" t="s">
         <v>758</v>
       </c>
@@ -21014,36 +21026,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="38" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A38" s="54"/>
-      <c r="B38" s="111" t="s">
+      <c r="B38" s="92" t="s">
         <v>761</v>
       </c>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="112"/>
-      <c r="N38" s="112"/>
-      <c r="O38" s="112"/>
-      <c r="P38" s="112"/>
-      <c r="Q38" s="112"/>
-      <c r="R38" s="112"/>
-      <c r="S38" s="112"/>
-      <c r="T38" s="112"/>
-      <c r="U38" s="112"/>
-      <c r="V38" s="112"/>
-      <c r="W38" s="112"/>
-      <c r="X38" s="112"/>
-      <c r="Y38" s="112"/>
-      <c r="Z38" s="112"/>
-      <c r="AA38" s="113"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="93"/>
+      <c r="O38" s="93"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="93"/>
+      <c r="T38" s="93"/>
+      <c r="U38" s="93"/>
+      <c r="V38" s="93"/>
+      <c r="W38" s="93"/>
+      <c r="X38" s="93"/>
+      <c r="Y38" s="93"/>
+      <c r="Z38" s="93"/>
+      <c r="AA38" s="94"/>
       <c r="AB38" s="56" t="s">
         <v>0</v>
       </c>
@@ -21207,7 +21219,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="43" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A43" s="54">
         <v>29</v>
       </c>
@@ -21246,36 +21258,36 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="44" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A44" s="54"/>
-      <c r="B44" s="111" t="s">
+      <c r="B44" s="92" t="s">
         <v>801</v>
       </c>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="112"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
-      <c r="K44" s="112"/>
-      <c r="L44" s="112"/>
-      <c r="M44" s="112"/>
-      <c r="N44" s="112"/>
-      <c r="O44" s="112"/>
-      <c r="P44" s="112"/>
-      <c r="Q44" s="112"/>
-      <c r="R44" s="112"/>
-      <c r="S44" s="112"/>
-      <c r="T44" s="112"/>
-      <c r="U44" s="112"/>
-      <c r="V44" s="112"/>
-      <c r="W44" s="112"/>
-      <c r="X44" s="112"/>
-      <c r="Y44" s="112"/>
-      <c r="Z44" s="112"/>
-      <c r="AA44" s="113"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="94"/>
       <c r="AB44" s="56" t="s">
         <v>802</v>
       </c>
@@ -21358,7 +21370,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="47" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A47" s="54">
         <v>32</v>
       </c>
@@ -21397,36 +21409,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="48" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A48" s="54"/>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="92" t="s">
         <v>810</v>
       </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="M48" s="112"/>
-      <c r="N48" s="112"/>
-      <c r="O48" s="112"/>
-      <c r="P48" s="112"/>
-      <c r="Q48" s="112"/>
-      <c r="R48" s="112"/>
-      <c r="S48" s="112"/>
-      <c r="T48" s="112"/>
-      <c r="U48" s="112"/>
-      <c r="V48" s="112"/>
-      <c r="W48" s="112"/>
-      <c r="X48" s="112"/>
-      <c r="Y48" s="112"/>
-      <c r="Z48" s="112"/>
-      <c r="AA48" s="113"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="93"/>
+      <c r="P48" s="93"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="93"/>
+      <c r="T48" s="93"/>
+      <c r="U48" s="93"/>
+      <c r="V48" s="93"/>
+      <c r="W48" s="93"/>
+      <c r="X48" s="93"/>
+      <c r="Y48" s="93"/>
+      <c r="Z48" s="93"/>
+      <c r="AA48" s="94"/>
       <c r="AB48" s="56" t="s">
         <v>814</v>
       </c>
@@ -21509,7 +21521,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="51" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A51" s="54">
         <v>35</v>
       </c>
@@ -21548,36 +21560,36 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="52" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A52" s="54"/>
-      <c r="B52" s="111" t="s">
+      <c r="B52" s="92" t="s">
         <v>821</v>
       </c>
-      <c r="C52" s="112"/>
-      <c r="D52" s="112"/>
-      <c r="E52" s="112"/>
-      <c r="F52" s="112"/>
-      <c r="G52" s="112"/>
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="112"/>
-      <c r="L52" s="112"/>
-      <c r="M52" s="112"/>
-      <c r="N52" s="112"/>
-      <c r="O52" s="112"/>
-      <c r="P52" s="112"/>
-      <c r="Q52" s="112"/>
-      <c r="R52" s="112"/>
-      <c r="S52" s="112"/>
-      <c r="T52" s="112"/>
-      <c r="U52" s="112"/>
-      <c r="V52" s="112"/>
-      <c r="W52" s="112"/>
-      <c r="X52" s="112"/>
-      <c r="Y52" s="112"/>
-      <c r="Z52" s="112"/>
-      <c r="AA52" s="113"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
+      <c r="K52" s="93"/>
+      <c r="L52" s="93"/>
+      <c r="M52" s="93"/>
+      <c r="N52" s="93"/>
+      <c r="O52" s="93"/>
+      <c r="P52" s="93"/>
+      <c r="Q52" s="93"/>
+      <c r="R52" s="93"/>
+      <c r="S52" s="93"/>
+      <c r="T52" s="93"/>
+      <c r="U52" s="93"/>
+      <c r="V52" s="93"/>
+      <c r="W52" s="93"/>
+      <c r="X52" s="93"/>
+      <c r="Y52" s="93"/>
+      <c r="Z52" s="93"/>
+      <c r="AA52" s="94"/>
       <c r="AB52" s="56" t="s">
         <v>820</v>
       </c>
@@ -21621,7 +21633,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="54" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A54" s="54">
         <v>37</v>
       </c>
@@ -21660,36 +21672,36 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="14.25" hidden="1" thickBot="1">
+    <row r="55" spans="1:28" ht="15.75" hidden="1" thickBot="1">
       <c r="A55" s="54"/>
-      <c r="B55" s="111" t="s">
+      <c r="B55" s="92" t="s">
         <v>818</v>
       </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="112"/>
-      <c r="L55" s="112"/>
-      <c r="M55" s="112"/>
-      <c r="N55" s="112"/>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
-      <c r="Q55" s="112"/>
-      <c r="R55" s="112"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="112"/>
-      <c r="U55" s="112"/>
-      <c r="V55" s="112"/>
-      <c r="W55" s="112"/>
-      <c r="X55" s="112"/>
-      <c r="Y55" s="112"/>
-      <c r="Z55" s="112"/>
-      <c r="AA55" s="113"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="93"/>
+      <c r="J55" s="93"/>
+      <c r="K55" s="93"/>
+      <c r="L55" s="93"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="93"/>
+      <c r="O55" s="93"/>
+      <c r="P55" s="93"/>
+      <c r="Q55" s="93"/>
+      <c r="R55" s="93"/>
+      <c r="S55" s="93"/>
+      <c r="T55" s="93"/>
+      <c r="U55" s="93"/>
+      <c r="V55" s="93"/>
+      <c r="W55" s="93"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="94"/>
       <c r="AB55" s="56" t="s">
         <v>819</v>
       </c>
@@ -21773,7 +21785,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="12" hidden="1" thickBot="1">
+    <row r="58" spans="1:28" ht="12.75" hidden="1" thickBot="1">
       <c r="A58" s="54">
         <f t="shared" si="12"/>
         <v>40</v>
@@ -21885,36 +21897,36 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="14.25" thickBot="1">
+    <row r="59" spans="1:28" ht="15.75" thickBot="1">
       <c r="A59" s="54"/>
-      <c r="B59" s="111" t="s">
-        <v>845</v>
-      </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="112"/>
-      <c r="E59" s="112"/>
-      <c r="F59" s="112"/>
-      <c r="G59" s="112"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="112"/>
-      <c r="L59" s="112"/>
-      <c r="M59" s="112"/>
-      <c r="N59" s="112"/>
-      <c r="O59" s="112"/>
-      <c r="P59" s="112"/>
-      <c r="Q59" s="112"/>
-      <c r="R59" s="112"/>
-      <c r="S59" s="112"/>
-      <c r="T59" s="112"/>
-      <c r="U59" s="112"/>
-      <c r="V59" s="112"/>
-      <c r="W59" s="112"/>
-      <c r="X59" s="112"/>
-      <c r="Y59" s="112"/>
-      <c r="Z59" s="112"/>
-      <c r="AA59" s="113"/>
+      <c r="B59" s="92" t="s">
+        <v>867</v>
+      </c>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="93"/>
+      <c r="F59" s="93"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="93"/>
+      <c r="J59" s="93"/>
+      <c r="K59" s="93"/>
+      <c r="L59" s="93"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="93"/>
+      <c r="O59" s="93"/>
+      <c r="P59" s="93"/>
+      <c r="Q59" s="93"/>
+      <c r="R59" s="93"/>
+      <c r="S59" s="93"/>
+      <c r="T59" s="93"/>
+      <c r="U59" s="93"/>
+      <c r="V59" s="93"/>
+      <c r="W59" s="93"/>
+      <c r="X59" s="93"/>
+      <c r="Y59" s="93"/>
+      <c r="Z59" s="93"/>
+      <c r="AA59" s="94"/>
       <c r="AB59" s="56" t="s">
         <v>854</v>
       </c>
@@ -22084,7 +22096,7 @@
         <v>42</v>
       </c>
       <c r="B64" s="78" t="s">
-        <v>848</v>
+        <v>868</v>
       </c>
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>
@@ -22124,7 +22136,7 @@
         <v>43</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>849</v>
+        <v>869</v>
       </c>
       <c r="C65" s="80"/>
       <c r="D65" s="80"/>
@@ -22164,7 +22176,7 @@
         <v>44</v>
       </c>
       <c r="B66" s="65" t="s">
-        <v>850</v>
+        <v>870</v>
       </c>
       <c r="C66" s="69"/>
       <c r="D66" s="69"/>
@@ -22238,90 +22250,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:80" ht="12" thickBot="1">
+    <row r="68" spans="1:80" ht="12.75" thickBot="1">
       <c r="A68" s="54"/>
       <c r="B68" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="C68" s="125" t="s">
+      <c r="C68" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="126"/>
-      <c r="E68" s="126"/>
-      <c r="F68" s="126"/>
-      <c r="G68" s="126"/>
-      <c r="H68" s="126"/>
-      <c r="I68" s="126"/>
-      <c r="J68" s="126"/>
-      <c r="K68" s="126"/>
-      <c r="L68" s="126"/>
-      <c r="M68" s="126"/>
-      <c r="N68" s="126"/>
-      <c r="O68" s="126"/>
-      <c r="P68" s="126"/>
-      <c r="Q68" s="126"/>
-      <c r="R68" s="126"/>
-      <c r="S68" s="126"/>
-      <c r="T68" s="126"/>
-      <c r="U68" s="126"/>
-      <c r="V68" s="126"/>
-      <c r="W68" s="126"/>
-      <c r="X68" s="126"/>
-      <c r="Y68" s="126"/>
-      <c r="Z68" s="126"/>
-      <c r="AA68" s="127"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="101"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="101"/>
+      <c r="O68" s="101"/>
+      <c r="P68" s="101"/>
+      <c r="Q68" s="101"/>
+      <c r="R68" s="101"/>
+      <c r="S68" s="101"/>
+      <c r="T68" s="101"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="101"/>
+      <c r="W68" s="101"/>
+      <c r="X68" s="101"/>
+      <c r="Y68" s="101"/>
+      <c r="Z68" s="101"/>
+      <c r="AA68" s="102"/>
       <c r="AB68" s="56"/>
     </row>
-    <row r="69" spans="1:80" ht="12" thickBot="1">
+    <row r="69" spans="1:80" ht="12.75" thickBot="1">
       <c r="B69" s="63"/>
-      <c r="C69" s="120"/>
-      <c r="D69" s="121"/>
-      <c r="E69" s="121"/>
-      <c r="F69" s="121"/>
-      <c r="G69" s="121"/>
-      <c r="H69" s="121"/>
-      <c r="I69" s="121"/>
-      <c r="J69" s="121"/>
-      <c r="K69" s="121"/>
-      <c r="L69" s="121"/>
-      <c r="M69" s="121"/>
-      <c r="N69" s="121"/>
-      <c r="O69" s="121"/>
-      <c r="P69" s="121"/>
-      <c r="Q69" s="121"/>
-      <c r="R69" s="121"/>
-      <c r="S69" s="121"/>
-      <c r="T69" s="121"/>
-      <c r="U69" s="121"/>
-      <c r="V69" s="121"/>
-      <c r="W69" s="121"/>
-      <c r="X69" s="121"/>
-      <c r="Y69" s="121"/>
-      <c r="Z69" s="121"/>
-      <c r="AA69" s="122"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="96"/>
+      <c r="F69" s="96"/>
+      <c r="G69" s="96"/>
+      <c r="H69" s="96"/>
+      <c r="I69" s="96"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="96"/>
+      <c r="M69" s="96"/>
+      <c r="N69" s="96"/>
+      <c r="O69" s="96"/>
+      <c r="P69" s="96"/>
+      <c r="Q69" s="96"/>
+      <c r="R69" s="96"/>
+      <c r="S69" s="96"/>
+      <c r="T69" s="96"/>
+      <c r="U69" s="96"/>
+      <c r="V69" s="96"/>
+      <c r="W69" s="96"/>
+      <c r="X69" s="96"/>
+      <c r="Y69" s="96"/>
+      <c r="Z69" s="96"/>
+      <c r="AA69" s="97"/>
       <c r="AB69" s="60"/>
       <c r="CB69" s="69"/>
     </row>
   </sheetData>
   <sheetProtection password="CC71" sheet="1" selectLockedCells="1"/>
   <mergeCells count="33">
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="B21:AA21"/>
-    <mergeCell ref="B59:AA59"/>
-    <mergeCell ref="C68:AA68"/>
-    <mergeCell ref="C69:AA69"/>
-    <mergeCell ref="B36:AA36"/>
-    <mergeCell ref="B38:AA38"/>
-    <mergeCell ref="B44:AA44"/>
-    <mergeCell ref="B48:AA48"/>
-    <mergeCell ref="B52:AA52"/>
-    <mergeCell ref="B55:AA55"/>
-    <mergeCell ref="B33:AA33"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="AA7:AA8"/>
     <mergeCell ref="B9:AA9"/>
@@ -22338,6 +22333,23 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="B21:AA21"/>
+    <mergeCell ref="B59:AA59"/>
+    <mergeCell ref="C68:AA68"/>
+    <mergeCell ref="C69:AA69"/>
+    <mergeCell ref="B36:AA36"/>
+    <mergeCell ref="B38:AA38"/>
+    <mergeCell ref="B44:AA44"/>
+    <mergeCell ref="B48:AA48"/>
+    <mergeCell ref="B52:AA52"/>
+    <mergeCell ref="B55:AA55"/>
+    <mergeCell ref="B33:AA33"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:Z18">
     <cfRule type="notContainsBlanks" dxfId="160" priority="144">
@@ -23078,18 +23090,18 @@
       <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.73046875" customWidth="1"/>
-    <col min="3" max="3" width="12.265625" customWidth="1"/>
-    <col min="4" max="4" width="20.86328125" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" customWidth="1"/>
-    <col min="6" max="6" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.73046875" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" customWidth="1"/>
-    <col min="10" max="10" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -28385,13 +28397,13 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.73046875" customWidth="1"/>
-    <col min="4" max="4" width="40.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.265625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -29547,12 +29559,12 @@
       <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="2" max="2" width="40.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -34391,21 +34403,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34429,27 +34441,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45088050-6D1C-4374-A6E1-B9B58326C08D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1ed6e237-7a44-4d6d-bfbc-e270d277b5ad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="dac3fa0a-9923-49c3-b4ba-df6390fa58ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F970A073-BA64-4372-95DC-98C3FFA83DDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45088050-6D1C-4374-A6E1-B9B58326C08D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1ed6e237-7a44-4d6d-bfbc-e270d277b5ad"/>
-    <ds:schemaRef ds:uri="dac3fa0a-9923-49c3-b4ba-df6390fa58ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>